<commit_message>
Checkin from Work Location
</commit_message>
<xml_diff>
--- a/DOC/Design/Fields_Mapping.xlsx
+++ b/DOC/Design/Fields_Mapping.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Values" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$G$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$H$53</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Values!$G$1:$H$143</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="247">
   <si>
     <t>Date Time</t>
   </si>
@@ -85,9 +85,6 @@
     <t>CaseID</t>
   </si>
   <si>
-    <t>Main</t>
-  </si>
-  <si>
     <t>All Tabs</t>
   </si>
   <si>
@@ -109,9 +106,6 @@
     <t>EPI ID</t>
   </si>
   <si>
-    <t>LabID</t>
-  </si>
-  <si>
     <t>Date of investigation</t>
   </si>
   <si>
@@ -133,9 +127,6 @@
     <t xml:space="preserve">Date of last vaccination </t>
   </si>
   <si>
-    <t>Dateoflast vaccination</t>
-  </si>
-  <si>
     <t>Source of information</t>
   </si>
   <si>
@@ -172,9 +163,6 @@
     <t>Date serology specimen collected</t>
   </si>
   <si>
-    <t>Date samplecollected</t>
-  </si>
-  <si>
     <t>Date recieved at the Laboratory</t>
   </si>
   <si>
@@ -734,6 +722,54 @@
   </si>
   <si>
     <t>Mab.Measles</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Measles</t>
+  </si>
+  <si>
+    <t>Sub_Organization</t>
+  </si>
+  <si>
+    <t>Dateoflast_vaccination</t>
+  </si>
+  <si>
+    <t>Measles_Epi_linked</t>
+  </si>
+  <si>
+    <t>Rubella_Epi_linked</t>
+  </si>
+  <si>
+    <t>Number_of_days_after_travel</t>
+  </si>
+  <si>
+    <t>Destination_of_travel</t>
+  </si>
+  <si>
+    <t>Date_samplecollected</t>
+  </si>
+  <si>
+    <t>Type_of_specimen</t>
+  </si>
+  <si>
+    <t>Measles_ELISA</t>
+  </si>
+  <si>
+    <t>Rubella_ELISA</t>
+  </si>
+  <si>
+    <t>FINAL_DIGNOSIS</t>
+  </si>
+  <si>
+    <t>Condition_of_specimen</t>
+  </si>
+  <si>
+    <t>EPI_ID</t>
+  </si>
+  <si>
+    <t>HomeAddress</t>
   </si>
 </sst>
 </file>
@@ -1084,10 +1120,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="B1:G53"/>
+  <dimension ref="B1:H53"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1095,34 +1132,35 @@
     <col min="3" max="3" width="31.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="2:7" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>17</v>
@@ -1131,30 +1169,30 @@
         <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="G3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
         <v>0</v>
       </c>
-      <c r="F4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>15</v>
       </c>
@@ -1165,33 +1203,33 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="G5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>7</v>
+        <v>231</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>231</v>
       </c>
       <c r="E6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="H6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -1202,13 +1240,13 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>15</v>
       </c>
@@ -1219,16 +1257,16 @@
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>130</v>
-      </c>
-      <c r="F8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G8" t="s">
+        <v>124</v>
+      </c>
+      <c r="H8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -1239,16 +1277,16 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>130</v>
-      </c>
-      <c r="F9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G9" t="s">
+        <v>124</v>
+      </c>
+      <c r="H9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>15</v>
       </c>
@@ -1259,36 +1297,36 @@
         <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>130</v>
-      </c>
-      <c r="F10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G10" t="s">
+        <v>124</v>
+      </c>
+      <c r="H10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>233</v>
       </c>
       <c r="E11" t="s">
-        <v>130</v>
-      </c>
-      <c r="F11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G11" t="s">
+        <v>124</v>
+      </c>
+      <c r="H11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -1296,16 +1334,16 @@
         <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>246</v>
       </c>
       <c r="E12" t="s">
-        <v>129</v>
-      </c>
-      <c r="F12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="G12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>15</v>
       </c>
@@ -1316,784 +1354,866 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>130</v>
-      </c>
-      <c r="F13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G13" t="s">
+        <v>124</v>
+      </c>
+      <c r="H13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>18</v>
+        <v>232</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
         <v>23</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>232</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F14" t="s">
+      <c r="D15" t="s">
+        <v>245</v>
+      </c>
+      <c r="E15" t="s">
+        <v>125</v>
+      </c>
+      <c r="G15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>232</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>232</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" t="s">
-        <v>129</v>
-      </c>
-      <c r="F15" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="G17" t="s">
+        <v>124</v>
+      </c>
+      <c r="H17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>232</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
+        <v>234</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>232</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" t="s">
-        <v>130</v>
-      </c>
-      <c r="F17" t="s">
-        <v>128</v>
-      </c>
-      <c r="G17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="G19" t="s">
+        <v>124</v>
+      </c>
+      <c r="H19" t="s">
         <v>34</v>
       </c>
-      <c r="E18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" t="s">
+    </row>
+    <row r="20" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>232</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
+        <v>235</v>
+      </c>
+      <c r="E20" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" t="s">
-        <v>130</v>
-      </c>
-      <c r="F19" t="s">
-        <v>128</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="G20" t="s">
+        <v>124</v>
+      </c>
+      <c r="H20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="3" t="s">
+    <row r="21" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>232</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" t="s">
-        <v>130</v>
-      </c>
-      <c r="F20" t="s">
-        <v>128</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="D21" t="s">
+        <v>236</v>
+      </c>
+      <c r="E21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G21" t="s">
+        <v>124</v>
+      </c>
+      <c r="H21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>232</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="D22" t="s">
+        <v>237</v>
+      </c>
+      <c r="E22" t="s">
+        <v>126</v>
+      </c>
+      <c r="G22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>232</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D23" t="s">
+        <v>238</v>
+      </c>
+      <c r="E23" t="s">
+        <v>125</v>
+      </c>
+      <c r="G23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>42</v>
       </c>
-      <c r="E21" t="s">
-        <v>130</v>
-      </c>
-      <c r="F21" t="s">
-        <v>128</v>
-      </c>
-      <c r="G21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" t="s">
-        <v>130</v>
-      </c>
-      <c r="F22" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="D24" t="s">
+        <v>239</v>
+      </c>
+      <c r="E24" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D23" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" t="s">
-        <v>129</v>
-      </c>
-      <c r="F23" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="D25" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="E25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="D26" t="s">
+        <v>240</v>
+      </c>
+      <c r="E26" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="G26" t="s">
+        <v>124</v>
+      </c>
+      <c r="H26" t="s">
         <v>48</v>
       </c>
-      <c r="D25" t="s">
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E25" t="s">
-        <v>24</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="D27" t="s">
+        <v>244</v>
+      </c>
+      <c r="E27" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="G27" t="s">
+        <v>124</v>
+      </c>
+      <c r="H27" t="s">
         <v>51</v>
       </c>
-      <c r="E26" t="s">
-        <v>130</v>
-      </c>
-      <c r="F26" t="s">
-        <v>128</v>
-      </c>
-      <c r="G26" t="s">
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="D28" t="s">
         <v>53</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E28" t="s">
+        <v>126</v>
+      </c>
+      <c r="G28" t="s">
+        <v>124</v>
+      </c>
+      <c r="H28" t="s">
         <v>54</v>
       </c>
-      <c r="E27" t="s">
-        <v>130</v>
-      </c>
-      <c r="F27" t="s">
-        <v>128</v>
-      </c>
-      <c r="G27" t="s">
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="D29" t="s">
         <v>56</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E29" t="s">
+        <v>126</v>
+      </c>
+      <c r="G29" t="s">
+        <v>124</v>
+      </c>
+      <c r="H29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E28" t="s">
-        <v>130</v>
-      </c>
-      <c r="F28" t="s">
-        <v>128</v>
-      </c>
-      <c r="G28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="3" t="s">
+      <c r="D30" t="s">
+        <v>241</v>
+      </c>
+      <c r="E30" t="s">
+        <v>126</v>
+      </c>
+      <c r="G30" t="s">
+        <v>124</v>
+      </c>
+      <c r="H30" t="s">
         <v>59</v>
       </c>
-      <c r="D29" t="s">
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E29" t="s">
-        <v>130</v>
-      </c>
-      <c r="F29" t="s">
-        <v>128</v>
-      </c>
-      <c r="G29" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
+        <v>242</v>
+      </c>
+      <c r="E31" t="s">
+        <v>126</v>
+      </c>
+      <c r="G31" t="s">
+        <v>124</v>
+      </c>
+      <c r="H31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E30" t="s">
-        <v>130</v>
-      </c>
-      <c r="F30" t="s">
-        <v>128</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="D32" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31" s="3" t="s">
+      <c r="E32" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" t="str">
+        <f>D32 &amp; "   " &amp; E32 &amp; ","</f>
+        <v>Datelabreportback   Date,</v>
+      </c>
+      <c r="G32" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>64</v>
       </c>
-      <c r="D31" t="s">
+      <c r="C33" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E31" t="s">
-        <v>130</v>
-      </c>
-      <c r="F31" t="s">
-        <v>128</v>
-      </c>
-      <c r="G31" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="D33" t="s">
         <v>66</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E33" t="s">
+        <v>126</v>
+      </c>
+      <c r="F33" t="str">
+        <f>D33 &amp; "   " &amp; E33 &amp; ","</f>
+        <v>Id_Source   Integer,</v>
+      </c>
+      <c r="G33" t="s">
+        <v>124</v>
+      </c>
+      <c r="H33" t="s">
         <v>67</v>
       </c>
-      <c r="E32" t="s">
-        <v>24</v>
-      </c>
-      <c r="F32" t="s">
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" t="s">
+        <v>243</v>
+      </c>
+      <c r="E34" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="F34" t="str">
+        <f>D34 &amp; "   " &amp; E34 &amp; ","</f>
+        <v>FINAL_DIGNOSIS   Integer,</v>
+      </c>
+      <c r="G34" t="s">
+        <v>124</v>
+      </c>
+      <c r="H34" t="s">
         <v>69</v>
       </c>
-      <c r="D33" t="s">
-        <v>70</v>
-      </c>
-      <c r="E33" t="s">
-        <v>130</v>
-      </c>
-      <c r="F33" t="s">
-        <v>128</v>
-      </c>
-      <c r="G33" t="s">
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="D35" t="s">
         <v>72</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E35" t="s">
+        <v>125</v>
+      </c>
+      <c r="F35" t="str">
+        <f>D35 &amp; "   " &amp; E35 &amp; ","</f>
+        <v>Reason_Sample_Sent2RL   String,</v>
+      </c>
+      <c r="G35" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" t="s">
         <v>74</v>
       </c>
-      <c r="E34" t="s">
-        <v>130</v>
-      </c>
-      <c r="F34" t="s">
-        <v>128</v>
-      </c>
-      <c r="G34" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>68</v>
-      </c>
-      <c r="C35" s="3" t="s">
+      <c r="E36" t="s">
+        <v>125</v>
+      </c>
+      <c r="F36" t="str">
+        <f>D36 &amp; "   " &amp; E36 &amp; ","</f>
+        <v>Type1stTest   String,</v>
+      </c>
+      <c r="G36" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D37" t="s">
         <v>76</v>
       </c>
-      <c r="E35" t="s">
-        <v>129</v>
-      </c>
-      <c r="F35" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>68</v>
-      </c>
-      <c r="C36" s="3" t="s">
+      <c r="E37" t="s">
+        <v>126</v>
+      </c>
+      <c r="F37" t="str">
+        <f>D37 &amp; "   " &amp; E37 &amp; ","</f>
+        <v>Type2ndSpecimen   Integer,</v>
+      </c>
+      <c r="G37" t="s">
+        <v>124</v>
+      </c>
+      <c r="H37" t="s">
         <v>77</v>
       </c>
-      <c r="D36" t="s">
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E36" t="s">
-        <v>129</v>
-      </c>
-      <c r="F36" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>68</v>
-      </c>
-      <c r="C37" s="3" t="s">
+      <c r="D38" t="s">
         <v>79</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E38" t="s">
+        <v>126</v>
+      </c>
+      <c r="F38" t="str">
+        <f>D38 &amp; "   " &amp; E38 &amp; ","</f>
+        <v>VG_Measles_RT-PCR   Integer,</v>
+      </c>
+      <c r="G38" t="s">
+        <v>124</v>
+      </c>
+      <c r="H38" t="s">
         <v>80</v>
       </c>
-      <c r="E37" t="s">
-        <v>130</v>
-      </c>
-      <c r="F37" t="s">
-        <v>128</v>
-      </c>
-      <c r="G37" t="s">
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>68</v>
-      </c>
-      <c r="C38" s="3" t="s">
+      <c r="D39" t="s">
         <v>82</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E39" t="s">
+        <v>126</v>
+      </c>
+      <c r="F39" t="str">
+        <f>D39 &amp; "   " &amp; E39 &amp; ","</f>
+        <v>VG_Rubella_RT-PCR   Integer,</v>
+      </c>
+      <c r="G39" t="s">
+        <v>124</v>
+      </c>
+      <c r="H39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E38" t="s">
-        <v>130</v>
-      </c>
-      <c r="F38" t="s">
-        <v>128</v>
-      </c>
-      <c r="G38" t="s">
+      <c r="D40" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>68</v>
-      </c>
-      <c r="C39" s="3" t="s">
+      <c r="E40" t="s">
+        <v>126</v>
+      </c>
+      <c r="F40" t="str">
+        <f>D40 &amp; "   " &amp; E40 &amp; ","</f>
+        <v>measles_genotype   Integer,</v>
+      </c>
+      <c r="G40" t="s">
+        <v>124</v>
+      </c>
+      <c r="H40" t="s">
         <v>85</v>
       </c>
-      <c r="D39" t="s">
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" t="s">
         <v>86</v>
       </c>
-      <c r="E39" t="s">
-        <v>130</v>
-      </c>
-      <c r="F39" t="s">
-        <v>128</v>
-      </c>
-      <c r="G39" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>68</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="E41" t="s">
+        <v>126</v>
+      </c>
+      <c r="F41" t="str">
+        <f>D41 &amp; "   " &amp; E41 &amp; ","</f>
+        <v>rubella_genotype   Integer,</v>
+      </c>
+      <c r="G41" t="s">
+        <v>124</v>
+      </c>
+      <c r="H41" t="s">
         <v>88</v>
       </c>
-      <c r="E40" t="s">
-        <v>130</v>
-      </c>
-      <c r="F40" t="s">
-        <v>128</v>
-      </c>
-      <c r="G40" t="s">
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>68</v>
-      </c>
-      <c r="C41" s="3" t="s">
+      <c r="D42" t="s">
+        <v>90</v>
+      </c>
+      <c r="E42" t="s">
+        <v>23</v>
+      </c>
+      <c r="F42" t="str">
+        <f>D42 &amp; "   " &amp; E42 &amp; ","</f>
+        <v>measles_date_sent_genotyping   Date,</v>
+      </c>
+      <c r="G42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D41" t="s">
-        <v>90</v>
-      </c>
-      <c r="E41" t="s">
-        <v>130</v>
-      </c>
-      <c r="F41" t="s">
-        <v>128</v>
-      </c>
-      <c r="G41" t="s">
+      <c r="D43" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="42" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>68</v>
-      </c>
-      <c r="C42" s="3" t="s">
+      <c r="E43" t="s">
+        <v>23</v>
+      </c>
+      <c r="F43" t="str">
+        <f>D43 &amp; "   " &amp; E43 &amp; ","</f>
+        <v>rubella_date_sent_genotyping   Date,</v>
+      </c>
+      <c r="G43" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>93</v>
       </c>
-      <c r="D42" t="s">
+      <c r="C44" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E42" t="s">
-        <v>24</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="D44" t="s">
+        <v>95</v>
+      </c>
+      <c r="E44" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="43" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="F44" t="str">
+        <f>D44 &amp; "   " &amp; E44 &amp; ","</f>
+        <v>Sero_Kit   Integer,</v>
+      </c>
+      <c r="G44" t="s">
+        <v>124</v>
+      </c>
+      <c r="H44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E43" t="s">
-        <v>24</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="D45" t="s">
+        <v>97</v>
+      </c>
+      <c r="E45" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>97</v>
-      </c>
-      <c r="C44" s="3" t="s">
+      <c r="F45" t="str">
+        <f>D45 &amp; "   " &amp; E45 &amp; ","</f>
+        <v>Sample_Sent2RL   Integer,</v>
+      </c>
+      <c r="G45" t="s">
+        <v>124</v>
+      </c>
+      <c r="H45" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D46" t="s">
         <v>99</v>
       </c>
-      <c r="E44" t="s">
-        <v>130</v>
-      </c>
-      <c r="F44" t="s">
-        <v>128</v>
-      </c>
-      <c r="G44" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>97</v>
-      </c>
-      <c r="C45" s="3" t="s">
+      <c r="E46" t="s">
+        <v>126</v>
+      </c>
+      <c r="F46" t="str">
+        <f>D46 &amp; "   " &amp; E46 &amp; ","</f>
+        <v>Sero_Measles_IgM   Integer,</v>
+      </c>
+      <c r="G46" t="s">
+        <v>124</v>
+      </c>
+      <c r="H46" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D47" t="s">
         <v>101</v>
       </c>
-      <c r="E45" t="s">
-        <v>130</v>
-      </c>
-      <c r="F45" t="s">
-        <v>128</v>
-      </c>
-      <c r="G45" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>97</v>
-      </c>
-      <c r="C46" s="3" t="s">
+      <c r="E47" t="s">
+        <v>126</v>
+      </c>
+      <c r="F47" t="str">
+        <f>D47 &amp; "   " &amp; E47 &amp; ","</f>
+        <v>Sero_Measles_IgG   Integer,</v>
+      </c>
+      <c r="G47" t="s">
+        <v>124</v>
+      </c>
+      <c r="H47" t="s">
         <v>102</v>
       </c>
-      <c r="D46" t="s">
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E46" t="s">
-        <v>130</v>
-      </c>
-      <c r="F46" t="s">
-        <v>128</v>
-      </c>
-      <c r="G46" t="s">
+      <c r="D48" t="s">
+        <v>104</v>
+      </c>
+      <c r="E48" t="s">
+        <v>126</v>
+      </c>
+      <c r="F48" t="str">
+        <f>D48 &amp; "   " &amp; E48 &amp; ","</f>
+        <v>Sero_Rubella_IgM   Integer,</v>
+      </c>
+      <c r="G48" t="s">
+        <v>124</v>
+      </c>
+      <c r="H48" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D49" t="s">
+        <v>107</v>
+      </c>
+      <c r="E49" t="s">
+        <v>126</v>
+      </c>
+      <c r="F49" t="str">
+        <f>D49 &amp; "   " &amp; E49 &amp; ","</f>
+        <v>Sero_Rubella_IgG   Integer,</v>
+      </c>
+      <c r="G49" t="s">
+        <v>124</v>
+      </c>
+      <c r="H49" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>93</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D50" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>97</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D47" t="s">
-        <v>105</v>
-      </c>
-      <c r="E47" t="s">
-        <v>130</v>
-      </c>
-      <c r="F47" t="s">
-        <v>128</v>
-      </c>
-      <c r="G47" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>97</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D48" t="s">
-        <v>108</v>
-      </c>
-      <c r="E48" t="s">
-        <v>130</v>
-      </c>
-      <c r="F48" t="s">
-        <v>128</v>
-      </c>
-      <c r="G48" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>97</v>
-      </c>
-      <c r="C49" s="3" t="s">
+      <c r="E50" t="s">
+        <v>126</v>
+      </c>
+      <c r="F50" t="str">
+        <f>D50 &amp; "   " &amp; E50 &amp; ","</f>
+        <v>IFA_Status   Integer,</v>
+      </c>
+      <c r="G50" t="s">
+        <v>124</v>
+      </c>
+      <c r="H50" t="s">
         <v>110</v>
       </c>
-      <c r="D49" t="s">
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E49" t="s">
-        <v>130</v>
-      </c>
-      <c r="F49" t="s">
-        <v>128</v>
-      </c>
-      <c r="G49" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>97</v>
-      </c>
-      <c r="C50" s="3" t="s">
+      <c r="D51" t="s">
         <v>112</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E51" t="s">
+        <v>126</v>
+      </c>
+      <c r="F51" t="str">
+        <f>D51 &amp; "   " &amp; E51 &amp; ","</f>
+        <v>VI_Vero_SLAM   Integer,</v>
+      </c>
+      <c r="G51" t="s">
+        <v>124</v>
+      </c>
+      <c r="H51" t="s">
         <v>113</v>
       </c>
-      <c r="E50" t="s">
-        <v>130</v>
-      </c>
-      <c r="F50" t="s">
-        <v>128</v>
-      </c>
-      <c r="G50" t="s">
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>97</v>
-      </c>
-      <c r="C51" s="3" t="s">
+      <c r="D52" t="s">
         <v>115</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E52" t="s">
+        <v>126</v>
+      </c>
+      <c r="F52" t="str">
+        <f>D52 &amp; "   " &amp; E52 &amp; ","</f>
+        <v>IFA   Integer,</v>
+      </c>
+      <c r="G52" t="s">
+        <v>124</v>
+      </c>
+      <c r="H52" t="s">
         <v>116</v>
       </c>
-      <c r="E51" t="s">
-        <v>130</v>
-      </c>
-      <c r="F51" t="s">
-        <v>128</v>
-      </c>
-      <c r="G51" t="s">
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>93</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>97</v>
-      </c>
-      <c r="C52" s="3" t="s">
+      <c r="D53" t="s">
         <v>118</v>
       </c>
-      <c r="D52" t="s">
-        <v>119</v>
-      </c>
-      <c r="E52" t="s">
-        <v>130</v>
-      </c>
-      <c r="F52" t="s">
-        <v>128</v>
-      </c>
-      <c r="G52" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>97</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D53" t="s">
-        <v>122</v>
-      </c>
       <c r="E53" t="s">
-        <v>130</v>
-      </c>
-      <c r="F53" t="s">
-        <v>128</v>
+        <v>126</v>
+      </c>
+      <c r="F53" t="str">
+        <f>D53 &amp; "   " &amp; E53 &amp; ","</f>
+        <v>VI_B95a   Integer,</v>
       </c>
       <c r="G53" t="s">
-        <v>117</v>
+        <v>124</v>
+      </c>
+      <c r="H53" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:G53">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Drop Down"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B1:H53"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2103,8 +2223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G1:K143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2116,10 +2236,10 @@
   <sheetData>
     <row r="1" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G1" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="7:11" x14ac:dyDescent="0.25">
@@ -2127,7 +2247,7 @@
         <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="J2" t="str">
         <f>"INSERT INTO [dbo].[lut_general_usages] VALUES ("""&amp;G2&amp;""" , """ &amp;H2&amp; """) "</f>
@@ -2143,7 +2263,7 @@
         <v>7</v>
       </c>
       <c r="H3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" ref="J3:J66" si="0">"INSERT INTO [dbo].[lut_general_usages] VALUES ("""&amp;G3&amp;""" , """ &amp;H3&amp; """) "</f>
@@ -2152,7 +2272,7 @@
     </row>
     <row r="4" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -2164,7 +2284,7 @@
     </row>
     <row r="5" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -2176,7 +2296,7 @@
     </row>
     <row r="6" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H6">
         <v>2</v>
@@ -2188,7 +2308,7 @@
     </row>
     <row r="7" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H7">
         <v>3</v>
@@ -2200,7 +2320,7 @@
     </row>
     <row r="8" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H8">
         <v>9</v>
@@ -2212,10 +2332,10 @@
     </row>
     <row r="9" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H9" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="0"/>
@@ -2224,10 +2344,10 @@
     </row>
     <row r="10" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H10" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="0"/>
@@ -2236,10 +2356,10 @@
     </row>
     <row r="11" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H11" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="0"/>
@@ -2248,10 +2368,10 @@
     </row>
     <row r="12" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H12" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="0"/>
@@ -2260,10 +2380,10 @@
     </row>
     <row r="13" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H13" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="0"/>
@@ -2272,10 +2392,10 @@
     </row>
     <row r="14" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H14" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="0"/>
@@ -2284,10 +2404,10 @@
     </row>
     <row r="15" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H15" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="0"/>
@@ -2296,10 +2416,10 @@
     </row>
     <row r="16" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H16" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="0"/>
@@ -2308,10 +2428,10 @@
     </row>
     <row r="17" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G17" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H17" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="0"/>
@@ -2320,10 +2440,10 @@
     </row>
     <row r="18" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H18" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="0"/>
@@ -2332,10 +2452,10 @@
     </row>
     <row r="19" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G19" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H19" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="0"/>
@@ -2344,10 +2464,10 @@
     </row>
     <row r="20" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H20" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="0"/>
@@ -2356,10 +2476,10 @@
     </row>
     <row r="21" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G21" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H21" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="0"/>
@@ -2368,10 +2488,10 @@
     </row>
     <row r="22" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G22" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H22" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="0"/>
@@ -2380,10 +2500,10 @@
     </row>
     <row r="23" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G23" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H23" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="0"/>
@@ -2392,10 +2512,10 @@
     </row>
     <row r="24" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G24" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H24" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="J24" t="str">
         <f t="shared" si="0"/>
@@ -2404,10 +2524,10 @@
     </row>
     <row r="25" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H25" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="0"/>
@@ -2416,10 +2536,10 @@
     </row>
     <row r="26" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G26" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H26" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="J26" t="str">
         <f t="shared" si="0"/>
@@ -2428,10 +2548,10 @@
     </row>
     <row r="27" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G27" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H27" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="J27" t="str">
         <f t="shared" si="0"/>
@@ -2440,10 +2560,10 @@
     </row>
     <row r="28" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G28" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H28" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="J28" t="str">
         <f t="shared" si="0"/>
@@ -2452,10 +2572,10 @@
     </row>
     <row r="29" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G29" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H29" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="J29" t="str">
         <f t="shared" si="0"/>
@@ -2464,10 +2584,10 @@
     </row>
     <row r="30" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G30" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H30" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="J30" t="str">
         <f t="shared" si="0"/>
@@ -2476,10 +2596,10 @@
     </row>
     <row r="31" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G31" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H31" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="J31" t="str">
         <f t="shared" si="0"/>
@@ -2488,10 +2608,10 @@
     </row>
     <row r="32" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H32" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="J32" t="str">
         <f t="shared" si="0"/>
@@ -2500,10 +2620,10 @@
     </row>
     <row r="33" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H33" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J33" t="str">
         <f t="shared" si="0"/>
@@ -2512,10 +2632,10 @@
     </row>
     <row r="34" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H34" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J34" t="str">
         <f t="shared" si="0"/>
@@ -2524,10 +2644,10 @@
     </row>
     <row r="35" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G35" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H35" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J35" t="str">
         <f t="shared" si="0"/>
@@ -2536,10 +2656,10 @@
     </row>
     <row r="36" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G36" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H36" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="J36" t="str">
         <f t="shared" si="0"/>
@@ -2548,10 +2668,10 @@
     </row>
     <row r="37" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H37" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="J37" t="str">
         <f t="shared" si="0"/>
@@ -2560,10 +2680,10 @@
     </row>
     <row r="38" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G38" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H38" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="J38" t="str">
         <f t="shared" si="0"/>
@@ -2572,10 +2692,10 @@
     </row>
     <row r="39" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G39" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H39" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="J39" t="str">
         <f t="shared" si="0"/>
@@ -2584,10 +2704,10 @@
     </row>
     <row r="40" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G40" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H40" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J40" t="str">
         <f t="shared" si="0"/>
@@ -2596,10 +2716,10 @@
     </row>
     <row r="41" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G41" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H41" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J41" t="str">
         <f t="shared" si="0"/>
@@ -2608,10 +2728,10 @@
     </row>
     <row r="42" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G42" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H42" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="J42" t="str">
         <f t="shared" si="0"/>
@@ -2620,10 +2740,10 @@
     </row>
     <row r="43" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G43" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H43" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="J43" t="str">
         <f t="shared" si="0"/>
@@ -2632,10 +2752,10 @@
     </row>
     <row r="44" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G44" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H44" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="J44" t="str">
         <f t="shared" si="0"/>
@@ -2644,10 +2764,10 @@
     </row>
     <row r="45" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G45" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H45" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="J45" t="str">
         <f t="shared" si="0"/>
@@ -2656,10 +2776,10 @@
     </row>
     <row r="46" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G46" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H46" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J46" t="str">
         <f t="shared" si="0"/>
@@ -2668,10 +2788,10 @@
     </row>
     <row r="47" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G47" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H47" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J47" t="str">
         <f t="shared" si="0"/>
@@ -2680,10 +2800,10 @@
     </row>
     <row r="48" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G48" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H48" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="J48" t="str">
         <f t="shared" si="0"/>
@@ -2692,10 +2812,10 @@
     </row>
     <row r="49" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G49" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H49" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J49" t="str">
         <f t="shared" si="0"/>
@@ -2704,10 +2824,10 @@
     </row>
     <row r="50" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G50" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H50" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="J50" t="str">
         <f t="shared" si="0"/>
@@ -2716,10 +2836,10 @@
     </row>
     <row r="51" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G51" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H51" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J51" t="str">
         <f t="shared" si="0"/>
@@ -2728,10 +2848,10 @@
     </row>
     <row r="52" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G52" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H52" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="J52" t="str">
         <f t="shared" si="0"/>
@@ -2740,10 +2860,10 @@
     </row>
     <row r="53" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G53" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H53" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="J53" t="str">
         <f t="shared" si="0"/>
@@ -2752,10 +2872,10 @@
     </row>
     <row r="54" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G54" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H54" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="J54" t="str">
         <f t="shared" si="0"/>
@@ -2764,10 +2884,10 @@
     </row>
     <row r="55" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G55" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H55" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J55" t="str">
         <f t="shared" si="0"/>
@@ -2776,10 +2896,10 @@
     </row>
     <row r="56" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G56" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H56" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="J56" t="str">
         <f t="shared" si="0"/>
@@ -2788,10 +2908,10 @@
     </row>
     <row r="57" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G57" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H57" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="J57" t="str">
         <f t="shared" si="0"/>
@@ -2800,10 +2920,10 @@
     </row>
     <row r="58" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G58" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H58" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="J58" t="str">
         <f t="shared" si="0"/>
@@ -2812,10 +2932,10 @@
     </row>
     <row r="59" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G59" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H59" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="J59" t="str">
         <f t="shared" si="0"/>
@@ -2824,10 +2944,10 @@
     </row>
     <row r="60" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G60" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H60" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="J60" t="str">
         <f t="shared" si="0"/>
@@ -2836,10 +2956,10 @@
     </row>
     <row r="61" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G61" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H61" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="J61" t="str">
         <f t="shared" si="0"/>
@@ -2848,10 +2968,10 @@
     </row>
     <row r="62" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G62" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H62" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="J62" t="str">
         <f t="shared" si="0"/>
@@ -2860,10 +2980,10 @@
     </row>
     <row r="63" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G63" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H63" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="J63" t="str">
         <f t="shared" si="0"/>
@@ -2872,10 +2992,10 @@
     </row>
     <row r="64" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G64" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H64" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="J64" t="str">
         <f t="shared" si="0"/>
@@ -2884,10 +3004,10 @@
     </row>
     <row r="65" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G65" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H65" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="J65" t="str">
         <f t="shared" si="0"/>
@@ -2896,10 +3016,10 @@
     </row>
     <row r="66" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G66" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H66" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="J66" t="str">
         <f t="shared" si="0"/>
@@ -2908,10 +3028,10 @@
     </row>
     <row r="67" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G67" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H67" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="J67" t="str">
         <f t="shared" ref="J67:J130" si="1">"INSERT INTO [dbo].[lut_general_usages] VALUES ("""&amp;G67&amp;""" , """ &amp;H67&amp; """) "</f>
@@ -2920,10 +3040,10 @@
     </row>
     <row r="68" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G68" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H68" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="J68" t="str">
         <f t="shared" si="1"/>
@@ -2932,10 +3052,10 @@
     </row>
     <row r="69" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G69" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H69" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="J69" t="str">
         <f t="shared" si="1"/>
@@ -2944,10 +3064,10 @@
     </row>
     <row r="70" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G70" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H70" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="J70" t="str">
         <f t="shared" si="1"/>
@@ -2956,10 +3076,10 @@
     </row>
     <row r="71" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G71" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H71" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="J71" t="str">
         <f t="shared" si="1"/>
@@ -2968,10 +3088,10 @@
     </row>
     <row r="72" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G72" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H72" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="J72" t="str">
         <f t="shared" si="1"/>
@@ -2980,10 +3100,10 @@
     </row>
     <row r="73" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G73" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H73" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J73" t="str">
         <f t="shared" si="1"/>
@@ -2992,10 +3112,10 @@
     </row>
     <row r="74" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G74" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H74" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="J74" t="str">
         <f t="shared" si="1"/>
@@ -3004,10 +3124,10 @@
     </row>
     <row r="75" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G75" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H75" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="J75" t="str">
         <f t="shared" si="1"/>
@@ -3016,10 +3136,10 @@
     </row>
     <row r="76" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G76" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H76" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="J76" t="str">
         <f t="shared" si="1"/>
@@ -3028,10 +3148,10 @@
     </row>
     <row r="77" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G77" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H77" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J77" t="str">
         <f t="shared" si="1"/>
@@ -3040,10 +3160,10 @@
     </row>
     <row r="78" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G78" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H78" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="J78" t="str">
         <f t="shared" si="1"/>
@@ -3052,10 +3172,10 @@
     </row>
     <row r="79" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G79" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H79" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J79" t="str">
         <f t="shared" si="1"/>
@@ -3064,10 +3184,10 @@
     </row>
     <row r="80" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G80" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H80" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="J80" t="str">
         <f t="shared" si="1"/>
@@ -3076,10 +3196,10 @@
     </row>
     <row r="81" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G81" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H81" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="J81" t="str">
         <f t="shared" si="1"/>
@@ -3088,10 +3208,10 @@
     </row>
     <row r="82" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G82" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H82" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="J82" t="str">
         <f t="shared" si="1"/>
@@ -3100,10 +3220,10 @@
     </row>
     <row r="83" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G83" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H83" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="J83" t="str">
         <f t="shared" si="1"/>
@@ -3112,10 +3232,10 @@
     </row>
     <row r="84" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G84" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H84" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="J84" t="str">
         <f t="shared" si="1"/>
@@ -3124,10 +3244,10 @@
     </row>
     <row r="85" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G85" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H85" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="J85" t="str">
         <f t="shared" si="1"/>
@@ -3136,10 +3256,10 @@
     </row>
     <row r="86" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G86" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H86" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="J86" t="str">
         <f t="shared" si="1"/>
@@ -3148,10 +3268,10 @@
     </row>
     <row r="87" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G87" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H87" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="J87" t="str">
         <f t="shared" si="1"/>
@@ -3160,10 +3280,10 @@
     </row>
     <row r="88" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G88" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H88" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="J88" t="str">
         <f t="shared" si="1"/>
@@ -3172,10 +3292,10 @@
     </row>
     <row r="89" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G89" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H89" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="J89" t="str">
         <f t="shared" si="1"/>
@@ -3184,10 +3304,10 @@
     </row>
     <row r="90" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G90" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H90" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="J90" t="str">
         <f t="shared" si="1"/>
@@ -3196,10 +3316,10 @@
     </row>
     <row r="91" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G91" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H91" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="J91" t="str">
         <f t="shared" si="1"/>
@@ -3208,10 +3328,10 @@
     </row>
     <row r="92" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G92" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H92" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="J92" t="str">
         <f t="shared" si="1"/>
@@ -3220,10 +3340,10 @@
     </row>
     <row r="93" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G93" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H93" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="J93" t="str">
         <f t="shared" si="1"/>
@@ -3232,10 +3352,10 @@
     </row>
     <row r="94" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G94" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H94" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="J94" t="str">
         <f t="shared" si="1"/>
@@ -3244,10 +3364,10 @@
     </row>
     <row r="95" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G95" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H95" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="J95" t="str">
         <f t="shared" si="1"/>
@@ -3256,10 +3376,10 @@
     </row>
     <row r="96" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G96" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H96" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="J96" t="str">
         <f t="shared" si="1"/>
@@ -3268,10 +3388,10 @@
     </row>
     <row r="97" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G97" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H97" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="J97" t="str">
         <f t="shared" si="1"/>
@@ -3280,10 +3400,10 @@
     </row>
     <row r="98" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G98" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H98" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="J98" t="str">
         <f t="shared" si="1"/>
@@ -3292,10 +3412,10 @@
     </row>
     <row r="99" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G99" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H99" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J99" t="str">
         <f t="shared" si="1"/>
@@ -3304,10 +3424,10 @@
     </row>
     <row r="100" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G100" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H100" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="J100" t="str">
         <f t="shared" si="1"/>
@@ -3316,10 +3436,10 @@
     </row>
     <row r="101" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G101" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H101" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="J101" t="str">
         <f t="shared" si="1"/>
@@ -3328,10 +3448,10 @@
     </row>
     <row r="102" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G102" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H102" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="J102" t="str">
         <f t="shared" si="1"/>
@@ -3340,10 +3460,10 @@
     </row>
     <row r="103" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G103" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H103" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="J103" t="str">
         <f t="shared" si="1"/>
@@ -3352,10 +3472,10 @@
     </row>
     <row r="104" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G104" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H104" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="J104" t="str">
         <f t="shared" si="1"/>
@@ -3364,10 +3484,10 @@
     </row>
     <row r="105" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G105" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H105" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="J105" t="str">
         <f t="shared" si="1"/>
@@ -3376,10 +3496,10 @@
     </row>
     <row r="106" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G106" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H106" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="J106" t="str">
         <f t="shared" si="1"/>
@@ -3388,10 +3508,10 @@
     </row>
     <row r="107" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G107" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H107" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="J107" t="str">
         <f t="shared" si="1"/>
@@ -3400,10 +3520,10 @@
     </row>
     <row r="108" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G108" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H108" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="J108" t="str">
         <f t="shared" si="1"/>
@@ -3412,10 +3532,10 @@
     </row>
     <row r="109" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G109" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H109" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="J109" t="str">
         <f t="shared" si="1"/>
@@ -3424,10 +3544,10 @@
     </row>
     <row r="110" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G110" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H110" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="J110" t="str">
         <f t="shared" si="1"/>
@@ -3436,10 +3556,10 @@
     </row>
     <row r="111" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G111" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H111" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="J111" t="str">
         <f t="shared" si="1"/>
@@ -3448,10 +3568,10 @@
     </row>
     <row r="112" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G112" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H112" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="J112" t="str">
         <f t="shared" si="1"/>
@@ -3460,10 +3580,10 @@
     </row>
     <row r="113" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G113" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H113" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J113" t="str">
         <f t="shared" si="1"/>
@@ -3472,10 +3592,10 @@
     </row>
     <row r="114" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G114" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H114" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="J114" t="str">
         <f t="shared" si="1"/>
@@ -3484,10 +3604,10 @@
     </row>
     <row r="115" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G115" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H115" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="J115" t="str">
         <f t="shared" si="1"/>
@@ -3496,10 +3616,10 @@
     </row>
     <row r="116" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G116" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H116" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="J116" t="str">
         <f t="shared" si="1"/>
@@ -3508,10 +3628,10 @@
     </row>
     <row r="117" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G117" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H117" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="J117" t="str">
         <f t="shared" si="1"/>
@@ -3520,10 +3640,10 @@
     </row>
     <row r="118" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G118" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H118" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="J118" t="str">
         <f t="shared" si="1"/>
@@ -3532,10 +3652,10 @@
     </row>
     <row r="119" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G119" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H119" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J119" t="str">
         <f t="shared" si="1"/>
@@ -3544,10 +3664,10 @@
     </row>
     <row r="120" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G120" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H120" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="J120" t="str">
         <f t="shared" si="1"/>
@@ -3556,10 +3676,10 @@
     </row>
     <row r="121" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G121" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H121" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="J121" t="str">
         <f t="shared" si="1"/>
@@ -3568,10 +3688,10 @@
     </row>
     <row r="122" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G122" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H122" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="J122" t="str">
         <f t="shared" si="1"/>
@@ -3580,10 +3700,10 @@
     </row>
     <row r="123" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G123" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H123" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="J123" t="str">
         <f t="shared" si="1"/>
@@ -3592,10 +3712,10 @@
     </row>
     <row r="124" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G124" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H124" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="J124" t="str">
         <f t="shared" si="1"/>
@@ -3604,10 +3724,10 @@
     </row>
     <row r="125" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G125" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H125" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="J125" t="str">
         <f t="shared" si="1"/>
@@ -3616,10 +3736,10 @@
     </row>
     <row r="126" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G126" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H126" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="J126" t="str">
         <f t="shared" si="1"/>
@@ -3628,10 +3748,10 @@
     </row>
     <row r="127" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G127" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H127" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="J127" t="str">
         <f t="shared" si="1"/>
@@ -3640,10 +3760,10 @@
     </row>
     <row r="128" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G128" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H128" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="J128" t="str">
         <f t="shared" si="1"/>
@@ -3652,10 +3772,10 @@
     </row>
     <row r="129" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G129" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H129" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="J129" t="str">
         <f t="shared" si="1"/>
@@ -3664,10 +3784,10 @@
     </row>
     <row r="130" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G130" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H130" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="J130" t="str">
         <f t="shared" si="1"/>
@@ -3676,10 +3796,10 @@
     </row>
     <row r="131" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G131" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H131" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="J131" t="str">
         <f t="shared" ref="J131:J143" si="2">"INSERT INTO [dbo].[lut_general_usages] VALUES ("""&amp;G131&amp;""" , """ &amp;H131&amp; """) "</f>
@@ -3688,10 +3808,10 @@
     </row>
     <row r="132" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G132" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H132" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="J132" t="str">
         <f t="shared" si="2"/>
@@ -3700,10 +3820,10 @@
     </row>
     <row r="133" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G133" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H133" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="J133" t="str">
         <f t="shared" si="2"/>
@@ -3712,10 +3832,10 @@
     </row>
     <row r="134" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G134" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H134" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="J134" t="str">
         <f t="shared" si="2"/>
@@ -3724,10 +3844,10 @@
     </row>
     <row r="135" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G135" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H135" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="J135" t="str">
         <f t="shared" si="2"/>
@@ -3736,10 +3856,10 @@
     </row>
     <row r="136" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G136" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H136" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="J136" t="str">
         <f t="shared" si="2"/>
@@ -3748,10 +3868,10 @@
     </row>
     <row r="137" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G137" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H137" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="J137" t="str">
         <f t="shared" si="2"/>
@@ -3760,10 +3880,10 @@
     </row>
     <row r="138" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G138" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H138" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="J138" t="str">
         <f t="shared" si="2"/>
@@ -3772,10 +3892,10 @@
     </row>
     <row r="139" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G139" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H139" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="J139" t="str">
         <f t="shared" si="2"/>
@@ -3784,10 +3904,10 @@
     </row>
     <row r="140" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G140" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H140" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="J140" t="str">
         <f t="shared" si="2"/>
@@ -3796,10 +3916,10 @@
     </row>
     <row r="141" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G141" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H141" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="J141" t="str">
         <f t="shared" si="2"/>
@@ -3808,10 +3928,10 @@
     </row>
     <row r="142" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G142" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H142" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="J142" t="str">
         <f t="shared" si="2"/>
@@ -3820,10 +3940,10 @@
     </row>
     <row r="143" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G143" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H143" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="J143" t="str">
         <f t="shared" si="2"/>

</xml_diff>